<commit_message>
Modified error correction scheme to be the minimization of the norm squared of the calculated coherency matrix and the unknown coherency matrix.  Also added a new function to handle plotting for each file provided to simplify the code
</commit_message>
<xml_diff>
--- a/HWP_hand_high.xlsx
+++ b/HWP_hand_high.xlsx
@@ -11,6 +11,7 @@
     <sheet name="calculated" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Adjusted" sheetId="3" state="visible" r:id="rId3"/>
     <sheet name="Adjusted2" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="rho" sheetId="5" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -1953,4 +1954,435 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>theta</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Jxx</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Jyy</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>beta</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>gamma</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>trace_sq</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
+        <v>0.00193466609378859</v>
+      </c>
+      <c r="C2" t="n">
+        <v>0.9980653681651108</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-0.0159222707822376</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.9966452594771784</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>5</v>
+      </c>
+      <c r="B3" t="n">
+        <v>0.03774810522500854</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0.9622518396249239</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-0.1905857933890676</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0.9999994115931092</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10</v>
+      </c>
+      <c r="B4" t="n">
+        <v>0.1317658986024291</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0.8682341433791049</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-0.3347319383646786</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.9952837208865037</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>0.2698379312570733</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.73016214786142</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-0.4356074999044452</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0.9854570592607016</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>20</v>
+      </c>
+      <c r="B6" t="n">
+        <v>0.4258182378288504</v>
+      </c>
+      <c r="C6" t="n">
+        <v>0.5741817461434889</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-0.4835477452990676</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.9786426932396772</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>25</v>
+      </c>
+      <c r="B7" t="n">
+        <v>0.6016459029625263</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.3983541098866221</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-0.4835001262464965</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.9882085335759128</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>30</v>
+      </c>
+      <c r="B8" t="n">
+        <v>0.7570303134257383</v>
+      </c>
+      <c r="C8" t="n">
+        <v>0.2429696919489803</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-0.4237348620356136</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0.9912316332599351</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>35</v>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8857858169408038</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.1142329877294931</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-0.3180972493350357</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F9" t="n">
+        <v>1.000037409048126</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>40</v>
+      </c>
+      <c r="B10" t="n">
+        <v>0.9712261945637656</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.02877422233326949</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-0.1671713270305639</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.000000782040017</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>45</v>
+      </c>
+      <c r="B11" t="n">
+        <v>0.9980284094936002</v>
+      </c>
+      <c r="C11" t="n">
+        <v>0.00197160076849049</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.001043480351031901</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9960667710684015</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>50</v>
+      </c>
+      <c r="B12" t="n">
+        <v>0.9624685513557465</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.03753156866800373</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.1737318873195663</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9881198683387473</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>55</v>
+      </c>
+      <c r="B13" t="n">
+        <v>0.8732650845918691</v>
+      </c>
+      <c r="C13" t="n">
+        <v>0.1267349424279521</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.3217522916708382</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.9857027279903331</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" t="n">
+        <v>0.7320320719302075</v>
+      </c>
+      <c r="C14" t="n">
+        <v>0.267968146975384</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.438943222663999</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.9930201875731675</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>65</v>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5788102362977725</v>
+      </c>
+      <c r="C15" t="n">
+        <v>0.4211898934090182</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.4918298635613694</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0.9962154453345737</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>70</v>
+      </c>
+      <c r="B16" t="n">
+        <v>0.4141676533940798</v>
+      </c>
+      <c r="C16" t="n">
+        <v>0.5858325329549383</v>
+      </c>
+      <c r="D16" t="n">
+        <v>0.4899534589677298</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0.9948433856952434</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>75</v>
+      </c>
+      <c r="B17" t="n">
+        <v>0.2498724551897367</v>
+      </c>
+      <c r="C17" t="n">
+        <v>0.75012761737949</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.4276994652928388</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.9909813514415378</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>80</v>
+      </c>
+      <c r="B18" t="n">
+        <v>0.1203202736650861</v>
+      </c>
+      <c r="C18" t="n">
+        <v>0.8796797687904249</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.3166513794355037</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0.9888496560708313</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>85</v>
+      </c>
+      <c r="B19" t="n">
+        <v>0.03209224622152107</v>
+      </c>
+      <c r="C19" t="n">
+        <v>0.9679080212922321</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.1653720777968055</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.9925716981790521</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>90</v>
+      </c>
+      <c r="B20" t="n">
+        <v>0.001897114660365675</v>
+      </c>
+      <c r="C20" t="n">
+        <v>0.9981028999871777</v>
+      </c>
+      <c r="D20" t="n">
+        <v>-0.01019143049454269</v>
+      </c>
+      <c r="E20" t="n">
+        <v>0</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0.9964207285178989</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
forgot to save new figures las time. also removed the old err_corr.py and the err_corr_stokes.py as they are no longer needed
</commit_message>
<xml_diff>
--- a/HWP_hand_high.xlsx
+++ b/HWP_hand_high.xlsx
@@ -2007,19 +2007,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.00193466609378859</v>
+        <v>0.002019505168937554</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9980653681651108</v>
+        <v>0.9979798498512131</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.0159222707822376</v>
+        <v>-0.01592065001370847</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9966452594771784</v>
+        <v>0.9964747933038952</v>
       </c>
     </row>
     <row r="3">
@@ -2027,19 +2027,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03774810522500854</v>
+        <v>0.03775121104179369</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9622518396249239</v>
+        <v>0.9622482864378208</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1905857933890676</v>
+        <v>-0.1905847500172665</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9999994115931092</v>
+        <v>0.9999920125659324</v>
       </c>
     </row>
     <row r="4">
@@ -2047,19 +2047,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1317658986024291</v>
+        <v>0.1317669245460725</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8682341433791049</v>
+        <v>0.8682276899384402</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.3347319383646786</v>
+        <v>-0.3347295139141208</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9952837208865037</v>
+        <v>0.9952695389505378</v>
       </c>
     </row>
     <row r="5">
@@ -2067,19 +2067,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2698379312570733</v>
+        <v>0.2698471110337028</v>
       </c>
       <c r="C5" t="n">
-        <v>0.73016214786142</v>
+        <v>0.7301526106211418</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4356074999044452</v>
+        <v>-0.4355967001524083</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9854570592607016</v>
+        <v>0.9854292684974385</v>
       </c>
     </row>
     <row r="6">
@@ -2087,19 +2087,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4258182378288504</v>
+        <v>0.4258164587174995</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5741817461434889</v>
+        <v>0.5741829257774871</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.4835477452990676</v>
+        <v>-0.4835647815288496</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9786426932396772</v>
+        <v>0.9786754846391954</v>
       </c>
     </row>
     <row r="7">
@@ -2107,19 +2107,19 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6016459029625263</v>
+        <v>0.6016475680482561</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3983541098866221</v>
+        <v>0.3983521804261683</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.4835001262464965</v>
+        <v>-0.4835133543444232</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9882085335759128</v>
+        <v>0.9882345834474551</v>
       </c>
     </row>
     <row r="8">
@@ -2127,19 +2127,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7570303134257383</v>
+        <v>0.7570344801606388</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2429696919489803</v>
+        <v>0.242965153778731</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.4237348620356136</v>
+        <v>-0.4237450773817907</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9912316332599351</v>
+        <v>0.9912530513134106</v>
       </c>
     </row>
     <row r="9">
@@ -2147,19 +2147,19 @@
         <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8857858169408038</v>
+        <v>0.8857694532051422</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1142329877294931</v>
+        <v>0.1142303747011243</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.3180972493350357</v>
+        <v>-0.3180906727165684</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1.000037409048126</v>
+        <v>0.999999454874254</v>
       </c>
     </row>
     <row r="10">
@@ -2167,19 +2167,19 @@
         <v>40</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9712261945637656</v>
+        <v>0.9712247978926558</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02877422233326949</v>
+        <v>0.02877509439310877</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1671713270305639</v>
+        <v>-0.167173473826011</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1.000000782040017</v>
+        <v>0.9999995548010744</v>
       </c>
     </row>
     <row r="11">
@@ -2187,19 +2187,19 @@
         <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9980284094936002</v>
+        <v>0.9979074051364609</v>
       </c>
       <c r="C11" t="n">
-        <v>0.00197160076849049</v>
+        <v>0.002092578668517589</v>
       </c>
       <c r="D11" t="n">
-        <v>0.001043480351031901</v>
+        <v>0.001043386063724748</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9960667710684015</v>
+        <v>0.9958257454206246</v>
       </c>
     </row>
     <row r="12">
@@ -2207,19 +2207,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9624685513557465</v>
+        <v>0.9624578348815204</v>
       </c>
       <c r="C12" t="n">
-        <v>0.03753156866800373</v>
+        <v>0.03754206072471921</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1737318873195663</v>
+        <v>0.1737275660453253</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9881198683387473</v>
+        <v>0.9880970246563483</v>
       </c>
     </row>
     <row r="13">
@@ -2227,19 +2227,19 @@
         <v>55</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8732650845918691</v>
+        <v>0.8732709381244274</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1267349424279521</v>
+        <v>0.1267290263756897</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3217522916708382</v>
+        <v>0.3217568091965035</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9857027279903331</v>
+        <v>0.9857172660274779</v>
       </c>
     </row>
     <row r="14">
@@ -2247,19 +2247,19 @@
         <v>60</v>
       </c>
       <c r="B14" t="n">
-        <v>0.7320320719302075</v>
+        <v>0.7320325802648044</v>
       </c>
       <c r="C14" t="n">
-        <v>0.267968146975384</v>
+        <v>0.2679670950812105</v>
       </c>
       <c r="D14" t="n">
-        <v>0.438943222663999</v>
+        <v>0.4389443617132359</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9930201875731675</v>
+        <v>0.99302236797509</v>
       </c>
     </row>
     <row r="15">
@@ -2267,19 +2267,19 @@
         <v>65</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5788102362977725</v>
+        <v>0.5787998687880876</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4211898934090182</v>
+        <v>0.4211995446830746</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4918298635613694</v>
+        <v>0.4917673561469877</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9962154453345737</v>
+        <v>0.9960886096939333</v>
       </c>
     </row>
     <row r="16">
@@ -2287,19 +2287,19 @@
         <v>70</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4141676533940798</v>
+        <v>0.4141706009673429</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5858325329549383</v>
+        <v>0.5858288293242142</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4899534589677298</v>
+        <v>0.4899343816007765</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9948433856952434</v>
+        <v>0.9948041005220998</v>
       </c>
     </row>
     <row r="17">
@@ -2307,19 +2307,19 @@
         <v>75</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2498724551897367</v>
+        <v>0.2498689946108097</v>
       </c>
       <c r="C17" t="n">
-        <v>0.75012761737949</v>
+        <v>0.7501308085203817</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4276994652928388</v>
+        <v>0.4277047569303205</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9909813514415378</v>
+        <v>0.9909934625609076</v>
       </c>
     </row>
     <row r="18">
@@ -2327,19 +2327,19 @@
         <v>80</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1203202736650861</v>
+        <v>0.1203110503589476</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8796797687904249</v>
+        <v>0.8796888577510674</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3166513794355037</v>
+        <v>0.3166586273697568</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9888496560708313</v>
+        <v>0.9888726078652479</v>
       </c>
     </row>
     <row r="19">
@@ -2347,19 +2347,19 @@
         <v>85</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03209224622152107</v>
+        <v>0.03208812392936315</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9679080212922321</v>
+        <v>0.967911609145745</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1653720777968055</v>
+        <v>0.1653730626948569</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9925716981790521</v>
+        <v>0.9925790305465658</v>
       </c>
     </row>
     <row r="20">
@@ -2367,19 +2367,19 @@
         <v>90</v>
       </c>
       <c r="B20" t="n">
-        <v>0.001897114660365675</v>
+        <v>0.001961610738810364</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9981028999871777</v>
+        <v>0.998038128551644</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.01019143049454269</v>
+        <v>-0.01019044392941942</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9964207285178989</v>
+        <v>0.9962916442545157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on adding the ability to find the maximum error epsilon for which the code still runs in order to obtain an idea of the worst case scenario
</commit_message>
<xml_diff>
--- a/HWP_hand_high.xlsx
+++ b/HWP_hand_high.xlsx
@@ -2007,19 +2007,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.002019505168937554</v>
+        <v>0.002008720035491786</v>
       </c>
       <c r="C2" t="n">
-        <v>0.9979798498512131</v>
+        <v>0.997991279964508</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01592065001370847</v>
+        <v>-0.01592100512942188</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9964747933038952</v>
+        <v>0.9964975866500401</v>
       </c>
     </row>
     <row r="3">
@@ -2027,19 +2027,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03775121104179369</v>
+        <v>0.03774874216183625</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9622482864378208</v>
+        <v>0.9622512578381636</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1905847500172665</v>
+        <v>-0.1905858715291551</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.9999920125659324</v>
+        <v>0.999998399598984</v>
       </c>
     </row>
     <row r="4">
@@ -2047,19 +2047,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1317669245460725</v>
+        <v>0.1317660722055312</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8682276899384402</v>
+        <v>0.8682339277944686</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.3347295139141208</v>
+        <v>-0.3347327364864055</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9952695389505378</v>
+        <v>0.9952844609092386</v>
       </c>
     </row>
     <row r="5">
@@ -2067,19 +2067,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2698471110337028</v>
+        <v>0.2698383726398281</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7301526106211418</v>
+        <v>0.7301616273601715</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4355967001524083</v>
+        <v>-0.4356135022051994</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9854292684974385</v>
+        <v>0.9854669960251233</v>
       </c>
     </row>
     <row r="6">
@@ -2087,19 +2087,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4258164587174995</v>
+        <v>0.4258165032635745</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5741829257774871</v>
+        <v>0.5741834967364258</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.4835647815288496</v>
+        <v>-0.4835664972448492</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9786754846391954</v>
+        <v>0.9786794968913923</v>
       </c>
     </row>
     <row r="7">
@@ -2107,19 +2107,19 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6016475680482561</v>
+        <v>0.6016498271326437</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3983521804261683</v>
+        <v>0.3983501728673565</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.4835133543444232</v>
+        <v>-0.4835235020363564</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9882345834474551</v>
+        <v>0.9882553287551974</v>
       </c>
     </row>
     <row r="8">
@@ -2127,19 +2127,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7570344801606388</v>
+        <v>0.7570346236636648</v>
       </c>
       <c r="C8" t="n">
-        <v>0.242965153778731</v>
+        <v>0.2429653763363355</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.4237450773817907</v>
+        <v>-0.4237450122174502</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9912530513134106</v>
+        <v>0.9912532662821778</v>
       </c>
     </row>
     <row r="9">
@@ -2147,19 +2147,19 @@
         <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8857694532051422</v>
+        <v>0.8857695945461598</v>
       </c>
       <c r="C9" t="n">
-        <v>0.1142303747011243</v>
+        <v>0.1142304054538406</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.3180906727165684</v>
+        <v>-0.3180907183099906</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.999999454874254</v>
+        <v>0.9999997703025487</v>
       </c>
     </row>
     <row r="10">
@@ -2167,19 +2167,19 @@
         <v>40</v>
       </c>
       <c r="B10" t="n">
-        <v>0.9712247978926558</v>
+        <v>0.971224865220418</v>
       </c>
       <c r="C10" t="n">
-        <v>0.02877509439310877</v>
+        <v>0.0287751347795822</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.167173473826011</v>
+        <v>-0.1671734786049066</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9999995548010744</v>
+        <v>0.9999996911017326</v>
       </c>
     </row>
     <row r="11">
@@ -2187,19 +2187,19 @@
         <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9979074051364609</v>
+        <v>0.9979019429187436</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002092578668517589</v>
+        <v>0.002098057081256728</v>
       </c>
       <c r="D11" t="n">
-        <v>0.001043386063724748</v>
+        <v>0.001043374600447599</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9958257454206246</v>
+        <v>0.9958148667856332</v>
       </c>
     </row>
     <row r="12">
@@ -2207,19 +2207,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9624578348815204</v>
+        <v>0.9624999050859196</v>
       </c>
       <c r="C12" t="n">
-        <v>0.03754206072471921</v>
+        <v>0.03750009491408049</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1737275660453253</v>
+        <v>0.1737433505878325</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9880970246563483</v>
+        <v>0.9881858281559424</v>
       </c>
     </row>
     <row r="13">
@@ -2227,19 +2227,19 @@
         <v>55</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8732709381244274</v>
+        <v>0.8733446416056645</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1267290263756897</v>
+        <v>0.1266553583943359</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3217568091965035</v>
+        <v>0.3218203257530738</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9857172660274779</v>
+        <v>0.9859090869669532</v>
       </c>
     </row>
     <row r="14">
@@ -2247,19 +2247,19 @@
         <v>60</v>
       </c>
       <c r="B14" t="n">
-        <v>0.7320325802648044</v>
+        <v>0.7320708129658005</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2679670950812105</v>
+        <v>0.2679291870342</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4389443617132359</v>
+        <v>0.4390163807560238</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.99302236797509</v>
+        <v>0.9931844896054515</v>
       </c>
     </row>
     <row r="15">
@@ -2267,19 +2267,19 @@
         <v>65</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5787998687880876</v>
+        <v>0.5788031245778535</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4211995446830746</v>
+        <v>0.4211968754221466</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4917673561469877</v>
+        <v>0.4917858443482729</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9960886096939333</v>
+        <v>0.9961264982891529</v>
       </c>
     </row>
     <row r="16">
@@ -2287,19 +2287,19 @@
         <v>70</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4141706009673429</v>
+        <v>0.4141724161681785</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5858288293242142</v>
+        <v>0.5858275838318215</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4899343816007765</v>
+        <v>0.4899256459936437</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9948041005220998</v>
+        <v>0.9947870254973949</v>
       </c>
     </row>
     <row r="17">
@@ -2307,19 +2307,19 @@
         <v>75</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2498689946108097</v>
+        <v>0.2498184174532385</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7501308085203817</v>
+        <v>0.7501815825467616</v>
       </c>
       <c r="D17" t="n">
-        <v>0.4277047569303205</v>
+        <v>0.427791408324233</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9909934625609076</v>
+        <v>0.9911926265632656</v>
       </c>
     </row>
     <row r="18">
@@ -2327,19 +2327,19 @@
         <v>80</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1203110503589476</v>
+        <v>0.1203005549793248</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8796888577510674</v>
+        <v>0.8796994450206753</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3166586273697568</v>
+        <v>0.3166674187812277</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9888726078652479</v>
+        <v>0.9888998453331487</v>
       </c>
     </row>
     <row r="19">
@@ -2347,19 +2347,19 @@
         <v>85</v>
       </c>
       <c r="B19" t="n">
-        <v>0.03208812392936315</v>
+        <v>0.031984641983513</v>
       </c>
       <c r="C19" t="n">
-        <v>0.967911609145745</v>
+        <v>0.9680153580164869</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1653730626948569</v>
+        <v>0.1654096832706021</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9925790305465658</v>
+        <v>0.9927974773179625</v>
       </c>
     </row>
     <row r="20">
@@ -2367,19 +2367,19 @@
         <v>90</v>
       </c>
       <c r="B20" t="n">
-        <v>0.001961610738810364</v>
+        <v>0.001844716687995392</v>
       </c>
       <c r="C20" t="n">
-        <v>0.998038128551644</v>
+        <v>0.9981552833120046</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.01019044392941942</v>
+        <v>-0.0101928383853115</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9962916442545157</v>
+        <v>0.9965251604920253</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished implemening an error optimization method for determining the worst case scenario in terms of error
</commit_message>
<xml_diff>
--- a/HWP_hand_high.xlsx
+++ b/HWP_hand_high.xlsx
@@ -2007,19 +2007,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>0.002008720035491786</v>
+        <v>0.002008720035500571</v>
       </c>
       <c r="C2" t="n">
-        <v>0.997991279964508</v>
+        <v>0.9979912799644994</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.01592100512942188</v>
+        <v>-0.01592100512942162</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>0.9964975866500401</v>
+        <v>0.9964975866500231</v>
       </c>
     </row>
     <row r="3">
@@ -2027,19 +2027,19 @@
         <v>5</v>
       </c>
       <c r="B3" t="n">
-        <v>0.03774874216183625</v>
+        <v>0.037748742161836</v>
       </c>
       <c r="C3" t="n">
-        <v>0.9622512578381636</v>
+        <v>0.962251257838164</v>
       </c>
       <c r="D3" t="n">
-        <v>-0.1905858715291551</v>
+        <v>-0.1905858715291553</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>0.999998399598984</v>
+        <v>0.999998399598985</v>
       </c>
     </row>
     <row r="4">
@@ -2047,19 +2047,19 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>0.1317660722055312</v>
+        <v>0.1317660722055272</v>
       </c>
       <c r="C4" t="n">
-        <v>0.8682339277944686</v>
+        <v>0.8682339277944726</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.3347327364864055</v>
+        <v>-0.3347327364864092</v>
       </c>
       <c r="E4" t="n">
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>0.9952844609092386</v>
+        <v>0.9952844609092494</v>
       </c>
     </row>
     <row r="5">
@@ -2067,19 +2067,19 @@
         <v>15</v>
       </c>
       <c r="B5" t="n">
-        <v>0.2698383726398281</v>
+        <v>0.2698383726398252</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7301616273601715</v>
+        <v>0.7301616273601746</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.4356135022051994</v>
+        <v>-0.4356135022052048</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>0.9854669960251233</v>
+        <v>0.9854669960251358</v>
       </c>
     </row>
     <row r="6">
@@ -2087,19 +2087,19 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>0.4258165032635745</v>
+        <v>0.4258165032635728</v>
       </c>
       <c r="C6" t="n">
-        <v>0.5741834967364258</v>
+        <v>0.5741834967364273</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.4835664972448492</v>
+        <v>-0.4835664972448601</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9786794968913923</v>
+        <v>0.9786794968914138</v>
       </c>
     </row>
     <row r="7">
@@ -2107,19 +2107,19 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>0.6016498271326437</v>
+        <v>0.6016498271326438</v>
       </c>
       <c r="C7" t="n">
-        <v>0.3983501728673565</v>
+        <v>0.3983501728673564</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.4835235020363564</v>
+        <v>-0.4835235020363571</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>0.9882553287551974</v>
+        <v>0.9882553287551991</v>
       </c>
     </row>
     <row r="8">
@@ -2127,19 +2127,19 @@
         <v>30</v>
       </c>
       <c r="B8" t="n">
-        <v>0.7570346236636648</v>
+        <v>0.7570346236636647</v>
       </c>
       <c r="C8" t="n">
-        <v>0.2429653763363355</v>
+        <v>0.2429653763363356</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.4237450122174502</v>
+        <v>-0.4237450122174501</v>
       </c>
       <c r="E8" t="n">
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>0.9912532662821778</v>
+        <v>0.9912532662821775</v>
       </c>
     </row>
     <row r="9">
@@ -2147,7 +2147,7 @@
         <v>35</v>
       </c>
       <c r="B9" t="n">
-        <v>0.8857695945461598</v>
+        <v>0.8857695945461597</v>
       </c>
       <c r="C9" t="n">
         <v>0.1142304054538406</v>
@@ -2159,7 +2159,7 @@
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>0.9999997703025487</v>
+        <v>0.9999997703025486</v>
       </c>
     </row>
     <row r="10">
@@ -2167,19 +2167,19 @@
         <v>40</v>
       </c>
       <c r="B10" t="n">
-        <v>0.971224865220418</v>
+        <v>0.9712248652204185</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0287751347795822</v>
+        <v>0.02877513477958181</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.1671734786049066</v>
+        <v>-0.1671734786049068</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>0.9999996911017326</v>
+        <v>0.9999996911017336</v>
       </c>
     </row>
     <row r="11">
@@ -2187,19 +2187,19 @@
         <v>45</v>
       </c>
       <c r="B11" t="n">
-        <v>0.9979019429187436</v>
+        <v>0.997901942918749</v>
       </c>
       <c r="C11" t="n">
-        <v>0.002098057081256728</v>
+        <v>0.002098057081251284</v>
       </c>
       <c r="D11" t="n">
-        <v>0.001043374600447599</v>
+        <v>0.001043374600447579</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>0.9958148667856332</v>
+        <v>0.995814866785644</v>
       </c>
     </row>
     <row r="12">
@@ -2207,19 +2207,19 @@
         <v>50</v>
       </c>
       <c r="B12" t="n">
-        <v>0.9624999050859196</v>
+        <v>0.9624999050859694</v>
       </c>
       <c r="C12" t="n">
-        <v>0.03750009491408049</v>
+        <v>0.037500094914031</v>
       </c>
       <c r="D12" t="n">
-        <v>0.1737433505878325</v>
+        <v>0.173743350587851</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>0.9881858281559424</v>
+        <v>0.9881858281560474</v>
       </c>
     </row>
     <row r="13">
@@ -2227,19 +2227,19 @@
         <v>55</v>
       </c>
       <c r="B13" t="n">
-        <v>0.8733446416056645</v>
+        <v>0.8733446416058365</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1266553583943359</v>
+        <v>0.1266553583941637</v>
       </c>
       <c r="D13" t="n">
-        <v>0.3218203257530738</v>
+        <v>0.3218203257532221</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>0.9859090869669532</v>
+        <v>0.985909086967401</v>
       </c>
     </row>
     <row r="14">
@@ -2247,19 +2247,19 @@
         <v>60</v>
       </c>
       <c r="B14" t="n">
-        <v>0.7320708129658005</v>
+        <v>0.7320708129657651</v>
       </c>
       <c r="C14" t="n">
-        <v>0.2679291870342</v>
+        <v>0.2679291870342352</v>
       </c>
       <c r="D14" t="n">
-        <v>0.4390163807560238</v>
+        <v>0.4390163807559569</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>0.9931844896054515</v>
+        <v>0.9931844896053013</v>
       </c>
     </row>
     <row r="15">
@@ -2267,19 +2267,19 @@
         <v>65</v>
       </c>
       <c r="B15" t="n">
-        <v>0.5788031245778535</v>
+        <v>0.5788031245778468</v>
       </c>
       <c r="C15" t="n">
-        <v>0.4211968754221466</v>
+        <v>0.4211968754221534</v>
       </c>
       <c r="D15" t="n">
-        <v>0.4917858443482729</v>
+        <v>0.4917858443482304</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>0.9961264982891529</v>
+        <v>0.9961264982890673</v>
       </c>
     </row>
     <row r="16">
@@ -2287,19 +2287,19 @@
         <v>70</v>
       </c>
       <c r="B16" t="n">
-        <v>0.4141724161681785</v>
+        <v>0.4141724161681772</v>
       </c>
       <c r="C16" t="n">
-        <v>0.5858275838318215</v>
+        <v>0.5858275838318229</v>
       </c>
       <c r="D16" t="n">
-        <v>0.4899256459936437</v>
+        <v>0.489925645993651</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
       </c>
       <c r="F16" t="n">
-        <v>0.9947870254973949</v>
+        <v>0.9947870254974096</v>
       </c>
     </row>
     <row r="17">
@@ -2307,19 +2307,19 @@
         <v>75</v>
       </c>
       <c r="B17" t="n">
-        <v>0.2498184174532385</v>
+        <v>0.2498184174532663</v>
       </c>
       <c r="C17" t="n">
-        <v>0.7501815825467616</v>
+        <v>0.7501815825467337</v>
       </c>
       <c r="D17" t="n">
-        <v>0.427791408324233</v>
+        <v>0.4277914083241852</v>
       </c>
       <c r="E17" t="n">
         <v>0</v>
       </c>
       <c r="F17" t="n">
-        <v>0.9911926265632656</v>
+        <v>0.9911926265631559</v>
       </c>
     </row>
     <row r="18">
@@ -2327,19 +2327,19 @@
         <v>80</v>
       </c>
       <c r="B18" t="n">
-        <v>0.1203005549793248</v>
+        <v>0.1203005549792871</v>
       </c>
       <c r="C18" t="n">
-        <v>0.8796994450206753</v>
+        <v>0.8796994450207132</v>
       </c>
       <c r="D18" t="n">
-        <v>0.3166674187812277</v>
+        <v>0.3166674187812594</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
       </c>
       <c r="F18" t="n">
-        <v>0.9888998453331487</v>
+        <v>0.9888998453332463</v>
       </c>
     </row>
     <row r="19">
@@ -2347,19 +2347,19 @@
         <v>85</v>
       </c>
       <c r="B19" t="n">
-        <v>0.031984641983513</v>
+        <v>0.03198464198350871</v>
       </c>
       <c r="C19" t="n">
-        <v>0.9680153580164869</v>
+        <v>0.9680153580164915</v>
       </c>
       <c r="D19" t="n">
-        <v>0.1654096832706021</v>
+        <v>0.1654096832706037</v>
       </c>
       <c r="E19" t="n">
         <v>0</v>
       </c>
       <c r="F19" t="n">
-        <v>0.9927974773179625</v>
+        <v>0.9927974773179723</v>
       </c>
     </row>
     <row r="20">
@@ -2367,19 +2367,19 @@
         <v>90</v>
       </c>
       <c r="B20" t="n">
-        <v>0.001844716687995392</v>
+        <v>0.001844716688017797</v>
       </c>
       <c r="C20" t="n">
-        <v>0.9981552833120046</v>
+        <v>0.9981552833119828</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.0101928383853115</v>
+        <v>-0.01019283838531107</v>
       </c>
       <c r="E20" t="n">
         <v>0</v>
       </c>
       <c r="F20" t="n">
-        <v>0.9965251604920253</v>
+        <v>0.9965251604919818</v>
       </c>
     </row>
   </sheetData>

</xml_diff>